<commit_message>
Did up basic Application.java
Can login and logout
However, I feel the login logic have something wrong
</commit_message>
<xml_diff>
--- a/database/Original/student list.xlsx
+++ b/database/Original/student list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\FYP system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryan/Documents/GitHub/SC2002---FYPMS/database/Original/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93015C6-51B2-494F-BF0D-6555A2297A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DC6E5C-DAFA-8A45-8663-64D7AC7105AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>AKY013@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -451,27 +454,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -479,7 +485,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -487,7 +493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -495,7 +501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -503,7 +509,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -511,7 +517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -519,7 +525,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -527,7 +533,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -535,7 +541,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -543,7 +549,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -551,7 +557,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>

</xml_diff>